<commit_message>
hide countries properties in kwargs to avoid breaking existing functions.
</commit_message>
<xml_diff>
--- a/tests/data/existing_ids.xlsx
+++ b/tests/data/existing_ids.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId1"/>
@@ -79,21 +79,89 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -663,7 +731,7 @@
       <c r="E9" s="3" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -679,9 +747,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>31.7.18</t>
@@ -694,7 +762,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -710,9 +778,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>version</t>
@@ -723,6 +791,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inline countries + id fix
</commit_message>
<xml_diff>
--- a/tests/data/existing_ids.xlsx
+++ b/tests/data/existing_ids.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId1"/>
@@ -79,89 +79,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -731,7 +663,7 @@
       <c r="E9" s="3" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -747,9 +679,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>31.7.18</t>
@@ -762,7 +694,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -778,9 +710,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>version</t>
@@ -791,6 +723,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>